<commit_message>
Added minder rettelser i brugermanual, rapport, go specifikationer. Tilføjet afsnit i Plan, samt kode i Ckoder
</commit_message>
<xml_diff>
--- a/Report/Tidsplan.xlsx
+++ b/Report/Tidsplan.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="40" windowWidth="24340" windowHeight="11720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Mål</t>
   </si>
   <si>
-    <t>Dage</t>
-  </si>
-  <si>
     <t>Delmål Basics</t>
   </si>
   <si>
@@ -79,13 +81,22 @@
   </si>
   <si>
     <t>Helpscreen, achievements</t>
+  </si>
+  <si>
+    <t>DEXXA Steering Wheel</t>
+  </si>
+  <si>
+    <t>Start Menu, Game Over, Game Won</t>
+  </si>
+  <si>
+    <t>Achievements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,8 +111,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,8 +155,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -123,17 +170,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,136 +568,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L11"/>
+  <dimension ref="A2:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -572,9 +955,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -584,8 +972,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>